<commit_message>
- documentation on Nexial Filter was wrong (or outdated). Fixed now. - updated unit test on compound filters.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_base_part2.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_base_part2.data.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11206"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-core/src/test/resources/showcase/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5B41A8-0683-B34E-A499-9C48E5D20107}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView tabRatio="500" windowHeight="20560" windowWidth="33600" xWindow="8380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-20560"/>
+    <workbookView xWindow="8380" yWindow="440" windowWidth="33600" windowHeight="20560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="#default" r:id="rId1" sheetId="2"/>
-    <sheet name="crypto" r:id="rId2" sheetId="4"/>
-    <sheet name="repeat-test" r:id="rId3" sheetId="5"/>
-    <sheet name="expression-test" r:id="rId4" sheetId="6"/>
-    <sheet name="multi-scenario1" r:id="rId5" sheetId="7"/>
-    <sheet name="multi-scenario2" r:id="rId6" sheetId="8"/>
+    <sheet name="#default" sheetId="2" r:id="rId1"/>
+    <sheet name="crypto" sheetId="4" r:id="rId2"/>
+    <sheet name="repeat-test" sheetId="5" r:id="rId3"/>
+    <sheet name="expression-test" sheetId="6" r:id="rId4"/>
+    <sheet name="multi-scenario1" sheetId="7" r:id="rId5"/>
+    <sheet name="multi-scenario2" sheetId="8" r:id="rId6"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
@@ -58,18 +59,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>sentry.pollWaitMs</t>
-  </si>
-  <si>
     <t>800</t>
-  </si>
-  <si>
-    <t>sentry.textDelim</t>
   </si>
   <si>
     <t>,</t>
@@ -81,31 +76,10 @@
     <t>var2</t>
   </si>
   <si>
-    <t>sentry.scope.mailTo</t>
-  </si>
-  <si>
-    <t>sentry.scope.executionMode</t>
-  </si>
-  <si>
     <t>local</t>
   </si>
   <si>
-    <t>sentry.scope.iteration</t>
-  </si>
-  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>sentry.scope.fallbackToPrevious</t>
-  </si>
-  <si>
-    <t>sentry.delayBetweenStepsMs</t>
-  </si>
-  <si>
-    <t>sentry.failFast</t>
-  </si>
-  <si>
-    <t>sentry.verbose</t>
   </si>
   <si>
     <t>false</t>
@@ -177,9 +151,6 @@
     <t>14</t>
   </si>
   <si>
-    <t>sentry.elapsedTimeSLA</t>
-  </si>
-  <si>
     <t>6000</t>
   </si>
   <si>
@@ -189,13 +160,7 @@
     <t>secretJane</t>
   </si>
   <si>
-    <t>crypt:4beafb332b5165ae0c6824feda3e88b80ab1a8fa5975ce63</t>
-  </si>
-  <si>
     <t>Cowabanga</t>
-  </si>
-  <si>
-    <t>sentry.scriptRef.startDate</t>
   </si>
   <si>
     <t>${startYear}-${startMonth}-${startDate}</t>
@@ -292,8 +257,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="23">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -368,84 +332,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="3E511F"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="287389"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="5A5A32"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="11.0"/>
-      <color rgb="12284A"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Consolas"/>
-      <sz val="10.0"/>
-      <color rgb="0000FF"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="050505"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="11.0"/>
-      <color rgb="006100"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="9C0006"/>
-      <b val="true"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Tahoma"/>
-      <sz val="10.0"/>
-      <color rgb="808080"/>
-      <u val="none"/>
-    </font>
   </fonts>
-  <fills count="26">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,127 +358,8 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="E6EFD7"/>
-        <bgColor rgb="E6EFD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="ECECE8"/>
-        <bgColor rgb="ECECE8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FAFAFA"/>
-        <bgColor rgb="FAFAFA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="F0F0E1"/>
-        <bgColor rgb="F0F0E1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF"/>
-        <bgColor rgb="FFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC7CE"/>
-        <bgColor rgb="FFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="C6EFCE"/>
-        <bgColor rgb="C6EFCE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="23">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -628,311 +397,81 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C8B4B4"/>
-      </left>
-      <right style="thin">
-        <color rgb="C8B4B4"/>
-      </right>
-      <top style="thin">
-        <color rgb="C8B4B4"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C8B4B4"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="DCDCDC"/>
-      </left>
-      <right style="thin">
-        <color rgb="DCDCDC"/>
-      </right>
-      <top style="thin">
-        <color rgb="DCDCDC"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="DCDCDC"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="CDCDCD"/>
-      </left>
-      <right style="thin">
-        <color rgb="CDCDCD"/>
-      </right>
-      <top style="thin">
-        <color rgb="CDCDCD"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="CDCDCD"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin"/>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="C3C3C3"/>
-      </left>
-      <right style="thin">
-        <color rgb="C3C3C3"/>
-      </right>
-      <top style="thin">
-        <color rgb="C3C3C3"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="C3C3C3"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="7" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0">
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyProtection="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyFont="1" applyProtection="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="5" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="3" fontId="8" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="0" fontId="9" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" applyProtection="1" borderId="2" fillId="4" fontId="10" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="10" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment indent="1" vertical="center" wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="18" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="4"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="6"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="8"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="10"/>
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="12"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="3"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="5"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="7"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="9"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="11"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="132">
     <dxf>
@@ -2744,7 +2283,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2763,7 +2302,7 @@
       <sheetName val="#system"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData refreshError="1" sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2774,10 +2313,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2812,7 +2351,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -2847,7 +2386,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -2941,21 +2480,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2972,7 +2511,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -3024,35 +2563,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAB21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AAA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -3757,7 +3296,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -4466,10 +4005,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -5175,7 +4714,7 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
@@ -5882,10 +5421,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -6591,10 +6130,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -7300,10 +6839,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -8009,10 +7548,10 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -8718,10 +8257,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -9427,10 +8966,10 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -10136,10 +9675,10 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -10845,14 +10384,14 @@
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C12"/>
       <c r="D12" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E12"/>
       <c r="F12"/>
@@ -11555,16 +11094,16 @@
     </row>
     <row r="13" spans="1:703">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E13"/>
       <c r="F13"/>
@@ -12267,16 +11806,16 @@
     </row>
     <row r="14" spans="1:703">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -12979,16 +12518,16 @@
     </row>
     <row r="15" spans="1:703">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E15"/>
       <c r="F15"/>
@@ -13691,13 +13230,13 @@
     </row>
     <row r="16" spans="1:703">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D16"/>
       <c r="E16"/>
@@ -14399,15 +13938,15 @@
       <c r="ZY16"/>
       <c r="ZZ16"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:702">
       <c r="A17" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D17"/>
       <c r="E17"/>
@@ -15109,15 +14648,15 @@
       <c r="ZY17"/>
       <c r="ZZ17"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:702">
       <c r="A18" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -15819,12 +15358,12 @@
       <c r="ZY18"/>
       <c r="ZZ18"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:702">
       <c r="A19" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -16527,12 +16066,12 @@
       <c r="ZY19"/>
       <c r="ZZ19"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:702">
       <c r="A20" s="1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -17235,12 +16774,12 @@
       <c r="ZY20"/>
       <c r="ZZ20"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:702">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -17944,118 +17483,118 @@
       <c r="ZZ21"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule dxfId="131" operator="beginsWith" priority="20" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="131" priority="20" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="130" operator="beginsWith" priority="21" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="130" priority="21" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="129" priority="22" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="129" priority="22" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B11 B15:B1048576">
-    <cfRule dxfId="128" priority="23" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="128" priority="23" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="127" priority="24" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="127" priority="24">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule dxfId="126" priority="18" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="126" priority="18" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="125" priority="19" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="125" priority="19">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule dxfId="124" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="124" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="123" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="123" priority="14">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="122" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="122" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="121" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="121" priority="12">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="120" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="120" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="119" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="119" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="118" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="118" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="117" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="117" priority="8">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="116" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="116" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="115" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="115" priority="6">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="114" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="114" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="113" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="113" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="112" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="112" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="111" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="111" priority="2">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AAB14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AAA14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="24.83203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="24.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -18760,10 +18299,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -19469,10 +19008,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -20219,115 +19758,115 @@
       <c r="B14" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A23:A1048576 A1:A19">
-    <cfRule dxfId="110" operator="beginsWith" priority="17" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="110" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="109" operator="beginsWith" priority="18" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="109" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="108" priority="19" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="108" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B11 B15:B1048576">
-    <cfRule dxfId="107" priority="20" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="107" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="106" priority="21" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="106" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule dxfId="105" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="105" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="104" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="104" priority="16">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule dxfId="103" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="103" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="102" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="102" priority="14">
       <formula>LEN(TRIM(B14))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="101" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="101" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="100" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="100" priority="12">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="99" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="99" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="98" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="98" priority="10">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="97" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="97" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="96" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="96" priority="8">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="95" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="95" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="94" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="94" priority="6">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="93" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="93" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="92" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="92" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="91" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="91" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="90" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="90" priority="2">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AAB13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AAA13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -21036,10 +20575,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -21745,7 +21284,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="6" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -22452,10 +21991,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -23161,10 +22700,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -23870,10 +23409,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -24579,10 +24118,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -25288,7 +24827,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -25997,10 +25536,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -26718,115 +26257,115 @@
       <c r="B13" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A22:A1048576 A1:A18">
-    <cfRule dxfId="89" operator="beginsWith" priority="17" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="89" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="88" operator="beginsWith" priority="18" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="88" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="87" priority="19" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="87" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B1048576 B1:B10">
-    <cfRule dxfId="86" priority="20" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="86" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="85" priority="21" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="85" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule dxfId="84" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="84" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="83" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="83" priority="16">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule dxfId="82" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="82" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="81" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="81" priority="14">
       <formula>LEN(TRIM(B13))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="80" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="80" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="79" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="79" priority="12">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="78" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="78" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="77" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="77" priority="10">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="76" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="76" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="75" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="75" priority="8">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="74" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="74" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="73" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="73" priority="6">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="72" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="72" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="71" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="71" priority="4">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="70" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="70" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="69" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="69" priority="2">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AAB12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:AAA12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -27535,10 +27074,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -28244,10 +27783,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -28953,10 +28492,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -29662,10 +29201,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -30371,10 +29910,10 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -31080,10 +30619,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -31805,118 +31344,118 @@
       <c r="B12" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A1:A17">
-    <cfRule dxfId="68" operator="beginsWith" priority="17" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="68" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="67" operator="beginsWith" priority="18" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="67" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="66" priority="19" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="66" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B1:B9">
-    <cfRule dxfId="65" priority="20" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="65" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="64" priority="21" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="64" priority="21">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule dxfId="63" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="63" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="62" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="62" priority="16">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="61" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="61" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="60" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="60" priority="14">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="59" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="59" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="58" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="58" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="57" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="57" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="56" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="56" priority="10">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="55" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="55" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="54" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="54" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="53" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="53" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="52" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="52" priority="6">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="51" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="51" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="50" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="50" priority="4">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="49" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="49" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="48" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="48" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AAB12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AAA12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -32622,10 +32161,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -33331,10 +32870,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -34040,10 +33579,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -34749,10 +34288,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -35458,7 +34997,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -36187,140 +35726,140 @@
       <c r="B12" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A1:A4 A7:A17">
-    <cfRule dxfId="47" operator="beginsWith" priority="23" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="47" priority="23" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="46" operator="beginsWith" priority="24" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="46" priority="24" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="45" priority="25" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="45" priority="25" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B1:B9">
-    <cfRule dxfId="44" priority="26" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="44" priority="26" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="43" priority="27" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="43" priority="27">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule dxfId="42" priority="21" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="42" priority="21" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="41" priority="22" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="41" priority="22">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="40" priority="19" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="40" priority="19" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="39" priority="20" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="39" priority="20">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="38" priority="17" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="38" priority="17" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="37" priority="18" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="37" priority="18">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="36" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="36" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="35" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="35" priority="16">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="34" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="34" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="33" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="33" priority="14">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="32" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="32" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="31" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="31" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="30" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="30" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="29" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="10">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="28" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="28" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="27" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule dxfId="26" operator="beginsWith" priority="4" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="26" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A5,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="25" operator="beginsWith" priority="5" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="25" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A5,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="24" priority="6" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="6" stopIfTrue="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule dxfId="23" operator="beginsWith" priority="1" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="23" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A6,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="22" operator="beginsWith" priority="2" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="22" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A6,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="21" priority="3" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A6))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AAB12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AAA12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="3" width="31.33203125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="3" width="28.83203125" collapsed="true"/>
-    <col min="4" max="27" customWidth="true" style="3" width="21.1640625" collapsed="true"/>
-    <col min="28" max="16384" style="3" width="10.83203125" collapsed="true"/>
+    <col min="1" max="1" width="31.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="9" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -37026,10 +36565,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -37735,10 +37274,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="9" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -38444,10 +37983,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="9" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -39153,10 +38692,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="11" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -39862,7 +39401,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="11" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -40591,91 +40130,91 @@
       <c r="B12" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection deleteColumns="0" deleteRows="0" insertColumns="0" insertRows="0"/>
+  <sheetProtection insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A21:A1048576 A7:A17">
-    <cfRule dxfId="20" operator="beginsWith" priority="17" stopIfTrue="1" text="sentry.scope." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="20" priority="17" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A7,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="19" operator="beginsWith" priority="18" stopIfTrue="1" text="sentry." type="beginsWith">
+    <cfRule type="beginsWith" dxfId="19" priority="18" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A7,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule dxfId="18" priority="19" stopIfTrue="1" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="19" stopIfTrue="1">
       <formula>LEN(TRIM(A7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B1048576 B5:B9">
-    <cfRule dxfId="17" priority="20" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="17" priority="20" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="16" priority="21" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="21">
       <formula>LEN(TRIM(B5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule dxfId="15" priority="15" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="14" priority="16" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="16">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule dxfId="13" priority="13" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="12" priority="14" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="14">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="11" priority="11" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="10" priority="12" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="12">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="9" priority="9" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="8" priority="10" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="8" priority="10">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="7" priority="7" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="6" priority="8" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="6" priority="8">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule dxfId="5" priority="5" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="4" priority="6" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="3" priority="3" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="2" priority="4" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="4">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule dxfId="1" priority="1" stopIfTrue="1" type="expression">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule dxfId="0" priority="2" type="notContainsBlanks">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Fixed failing unit test
Signed-off-by: akshay2409 <akki.kore24@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/unittesting/artifact/data/unitTest_base_part2.data.xlsx
+++ b/src/test/resources/unittesting/artifact/data/unitTest_base_part2.data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/unittesting/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nexial-Project\git\nexial-core\src\test\resources\unittesting\artifact\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB7A958-0101-0343-A25D-4CDF3ABC5088}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8380" yWindow="460" windowWidth="33600" windowHeight="20560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8385" yWindow="465" windowWidth="33600" windowHeight="20565" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -49,7 +48,7 @@
   <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -151,9 +150,6 @@
     <t>14</t>
   </si>
   <si>
-    <t>6000</t>
-  </si>
-  <si>
     <t>plainJane</t>
   </si>
   <si>
@@ -252,11 +248,14 @@
   <si>
     <t>nexial.mailTo</t>
   </si>
+  <si>
+    <t>12000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="11">
     <font>
       <sz val="12"/>
@@ -2570,23 +2569,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AAA21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="31.375" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="3" max="3" width="28.875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>5</v>
@@ -3294,7 +3295,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -4003,7 +4004,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>28</v>
@@ -4712,7 +4713,7 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4"/>
       <c r="C4"/>
@@ -5419,10 +5420,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -6128,7 +6129,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -6837,10 +6838,10 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -7546,7 +7547,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>2</v>
@@ -8255,7 +8256,7 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -15358,10 +15359,10 @@
     </row>
     <row r="19" spans="1:702">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="C19"/>
       <c r="D19"/>
@@ -16066,10 +16067,10 @@
     </row>
     <row r="20" spans="1:702">
       <c r="A20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -16774,10 +16775,10 @@
     </row>
     <row r="21" spans="1:702">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -17571,28 +17572,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AAA14"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="24.875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="3" max="3" width="28.875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -18297,10 +18298,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -19006,7 +19007,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>6</v>
@@ -19846,25 +19847,25 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AAA13"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="31.375" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="3" max="3" width="28.875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -20573,7 +20574,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -21282,7 +21283,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -21989,7 +21990,7 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -22698,7 +22699,7 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -23407,7 +23408,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
@@ -24116,7 +24117,7 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
@@ -24825,7 +24826,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>0</v>
@@ -25534,10 +25535,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -26345,25 +26346,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AAA12"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="31.375" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="3" max="3" width="28.875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -27072,7 +27073,7 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -27781,7 +27782,7 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -28490,7 +28491,7 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -29199,7 +29200,7 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>1</v>
@@ -29908,7 +29909,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>2</v>
@@ -30617,7 +30618,7 @@
     </row>
     <row r="7" spans="1:703">
       <c r="A7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -31432,28 +31433,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AAA12"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="31.375" style="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="3" max="3" width="28.875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -32159,10 +32160,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -32868,10 +32869,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -33577,10 +33578,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -34286,10 +34287,10 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -34995,7 +34996,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>
@@ -35836,28 +35837,28 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AAA12"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" style="3" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="31.375" style="3" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="36" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="28.83203125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+    <col min="3" max="3" width="28.875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="27" width="21.125" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.875" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -36563,10 +36564,10 @@
     </row>
     <row r="2" spans="1:703">
       <c r="A2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -37272,10 +37273,10 @@
     </row>
     <row r="3" spans="1:703">
       <c r="A3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -37981,10 +37982,10 @@
     </row>
     <row r="4" spans="1:703">
       <c r="A4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -38690,7 +38691,7 @@
     </row>
     <row r="5" spans="1:703">
       <c r="A5" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>28</v>
@@ -39399,7 +39400,7 @@
     </row>
     <row r="6" spans="1:703">
       <c r="A6" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>0</v>

</xml_diff>